<commit_message>
Tablero renderizando. Avance hasta valueboxes con cantidad de personas encuestadas. Filtro del año malo
</commit_message>
<xml_diff>
--- a/Tablero encuestas de satisfacción/Encuesta de satisfacción del servicio de transporte.xlsx
+++ b/Tablero encuestas de satisfacción/Encuesta de satisfacción del servicio de transporte.xlsx
@@ -1,26 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27823"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\Trabajo Sofi\UPN\Informes de escuestas de satisfacción\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DA4CA53-4268-491E-9D5F-BED41636CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BABE7047-C8DF-4791-98A5-98AD245F3E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{23EB98BE-3D12-49F5-AFA8-144FCFF6F0FB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Encuesta de satisfacción del se" sheetId="1" r:id="rId1"/>
+    <sheet name="Form1" sheetId="1" r:id="rId1"/>
+    <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_56F9DC9755BA473782653E2940F9FormId">"nGREgiPT_k6Tg1M4a_CM6ISJUD-DI7NBoIgAQxXYz_hUMTdPVkhHNklaVjdQQjcyVFZFS0kwNlFTMSQlQCN0PWcu"</definedName>
+    <definedName name="_56F9DC9755BA473782653E2940F9ResponseSheet">"Form1"</definedName>
+    <definedName name="_56F9DC9755BA473782653E2940F9SourceDocId">"{e23544ea-7b9b-4957-ba48-7e2c5253e036}"</definedName>
+  </definedNames>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -155,7 +177,13 @@
     <t>Edinson Nuñez Navia</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Manifiesto mi inconformidad por la forma como fue brindado el servicio respecto de la falta de empatía por parte de conductor con las personas que requieren el servicio institucional, ya que solicitaron bajar las cajas de manera inmediata dejándolas en el parqueadero expuestas al agua</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>Considero necesario fortalecer la competencia de trabajo en equipo y compromiso institucional</t>
@@ -174,12 +202,6 @@
     <t>Considero que el conductor debe fortalecer competencias como el trabajo en equipo y compromiso institucional</t>
   </si>
   <si>
-    <t>5/17/24 15:24:35</t>
-  </si>
-  <si>
-    <t>5/17/24 15:30:05</t>
-  </si>
-  <si>
     <t>vaheredia@pedagogica.edu.co</t>
   </si>
   <si>
@@ -201,15 +223,15 @@
     <t xml:space="preserve">Victor Andrés Heredia Heredia </t>
   </si>
   <si>
-    <t>5/17/2024</t>
-  </si>
-  <si>
     <t>Salida de campo</t>
   </si>
   <si>
     <t>Yohan Gabriel Montoya Hernández</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Todo se cumplió segun el itinerario y las necesidades del a salida </t>
   </si>
   <si>
@@ -219,12 +241,6 @@
     <t xml:space="preserve">El servicio se transporte cumplió con más expectativas </t>
   </si>
   <si>
-    <t>5/17/24 17:40:08</t>
-  </si>
-  <si>
-    <t>5/17/24 17:45:45</t>
-  </si>
-  <si>
     <t>fiespitiac@upn.edu.co</t>
   </si>
   <si>
@@ -249,12 +265,6 @@
     <t>Ninguno</t>
   </si>
   <si>
-    <t>5/18/24 15:22:54</t>
-  </si>
-  <si>
-    <t>5/18/24 15:26:02</t>
-  </si>
-  <si>
     <t>svmahecham@pedagogica.edu.co</t>
   </si>
   <si>
@@ -279,12 +289,6 @@
     <t>Es un conductor que presta un excelente servicio.</t>
   </si>
   <si>
-    <t>5/18/24 17:04:45</t>
-  </si>
-  <si>
-    <t>5/18/24 17:07:26</t>
-  </si>
-  <si>
     <t>jatorres@pedagogica.edu.co</t>
   </si>
   <si>
@@ -297,15 +301,6 @@
     <t>Johan Torres Cotrino</t>
   </si>
   <si>
-    <t>5/18/2024</t>
-  </si>
-  <si>
-    <t>5/20/24 11:30:19</t>
-  </si>
-  <si>
-    <t>5/20/24 11:33:48</t>
-  </si>
-  <si>
     <t>gecortest@upn.edu.co</t>
   </si>
   <si>
@@ -321,18 +316,9 @@
     <t xml:space="preserve">Gladys Cortes </t>
   </si>
   <si>
-    <t>5/20/2024</t>
-  </si>
-  <si>
     <t>Wilson Salazar Duque</t>
   </si>
   <si>
-    <t>5/21/24 8:53:39</t>
-  </si>
-  <si>
-    <t>5/21/24 8:55:21</t>
-  </si>
-  <si>
     <t>jsvillamizarm@upn.edu.co</t>
   </si>
   <si>
@@ -348,18 +334,9 @@
     <t>Johan Villamizar</t>
   </si>
   <si>
-    <t>5/21/2024</t>
-  </si>
-  <si>
     <t>Néstor Raúl Acosta</t>
   </si>
   <si>
-    <t>5/21/24 17:12:46</t>
-  </si>
-  <si>
-    <t>5/21/24 17:19:23</t>
-  </si>
-  <si>
     <t>hlguzmans@pedagogica.edu.co</t>
   </si>
   <si>
@@ -369,9 +346,6 @@
     <t xml:space="preserve">Martha Jeaneth García Sarmiento </t>
   </si>
   <si>
-    <t>5/14/2024</t>
-  </si>
-  <si>
     <t>Roland Alexander Niño Trujillo</t>
   </si>
   <si>
@@ -384,12 +358,6 @@
     <t>Ninguna. El servicio se prestó a cabalidad y se cumplió el itinerario previsto.</t>
   </si>
   <si>
-    <t>5/23/24 9:40:41</t>
-  </si>
-  <si>
-    <t>5/23/24 9:45:59</t>
-  </si>
-  <si>
     <t>eballesteros@pedagogica.edu.co</t>
   </si>
   <si>
@@ -402,18 +370,9 @@
     <t xml:space="preserve">Edilson Ballesteros </t>
   </si>
   <si>
-    <t>5/23/2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Excelente servicio </t>
   </si>
   <si>
-    <t>5/23/24 16:47:43</t>
-  </si>
-  <si>
-    <t>5/23/24 16:51:01</t>
-  </si>
-  <si>
     <t>danza_folclorica@upn.edu.co</t>
   </si>
   <si>
@@ -438,12 +397,6 @@
     <t xml:space="preserve">Excelente </t>
   </si>
   <si>
-    <t>5/24/24 12:11:31</t>
-  </si>
-  <si>
-    <t>5/24/24 12:14:15</t>
-  </si>
-  <si>
     <t>rgonzalezl@pedagogica.edu.co</t>
   </si>
   <si>
@@ -456,12 +409,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>5/24/24 12:32:54</t>
-  </si>
-  <si>
-    <t>5/24/24 12:36:33</t>
-  </si>
-  <si>
     <t>sst@pedagogica.edu.co</t>
   </si>
   <si>
@@ -474,15 +421,6 @@
     <t xml:space="preserve">Jessica Páez </t>
   </si>
   <si>
-    <t>5/24/2024</t>
-  </si>
-  <si>
-    <t>5/28/24 10:00:59</t>
-  </si>
-  <si>
-    <t>5/28/24 10:09:02</t>
-  </si>
-  <si>
     <t>cmhernandezr@pedagogica.edu.co</t>
   </si>
   <si>
@@ -495,21 +433,12 @@
     <t xml:space="preserve">Claudia Hernández </t>
   </si>
   <si>
-    <t>5/16/2024</t>
-  </si>
-  <si>
     <t>Salida administrativa</t>
   </si>
   <si>
     <t>Luis Fernando Castro</t>
   </si>
   <si>
-    <t>5/29/24 18:32:06</t>
-  </si>
-  <si>
-    <t>5/29/24 18:39:45</t>
-  </si>
-  <si>
     <t>bandasinfonica@upn.edu.co</t>
   </si>
   <si>
@@ -525,21 +454,12 @@
     <t>Oscar Vargas</t>
   </si>
   <si>
-    <t>5/29/2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Buen servicio </t>
   </si>
   <si>
     <t>Buen servicio</t>
   </si>
   <si>
-    <t>5/30/24 12:45:44</t>
-  </si>
-  <si>
-    <t>5/30/24 12:51:25</t>
-  </si>
-  <si>
     <t>mgilc@upn.edu.co</t>
   </si>
   <si>
@@ -555,9 +475,6 @@
     <t xml:space="preserve">Mónica Gil Cardona </t>
   </si>
   <si>
-    <t>5/30/2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Excelente servicio, actitud, colaboración y puntualidad en los recorridos. </t>
   </si>
   <si>
@@ -567,12 +484,6 @@
     <t xml:space="preserve">Grscias por el apoyo y compromiso </t>
   </si>
   <si>
-    <t>5/30/24 14:01:24</t>
-  </si>
-  <si>
-    <t>5/30/24 14:03:48</t>
-  </si>
-  <si>
     <t>wfosoriop@upn.edu.co</t>
   </si>
   <si>
@@ -588,12 +499,6 @@
     <t>Mejoro sustancialmente el servicio de transporte con respecto al año anterior</t>
   </si>
   <si>
-    <t>5/31/24 11:00:10</t>
-  </si>
-  <si>
-    <t>5/31/24 11:02:18</t>
-  </si>
-  <si>
     <t>madelahozm@upn.edu.co</t>
   </si>
   <si>
@@ -603,18 +508,9 @@
     <t>Mónica gil</t>
   </si>
   <si>
-    <t>5/31/2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exelente </t>
   </si>
   <si>
-    <t>5/31/24 11:54:42</t>
-  </si>
-  <si>
-    <t>5/31/24 12:00:00</t>
-  </si>
-  <si>
     <t>mimoscosop@pedagogica.edu.co</t>
   </si>
   <si>
@@ -633,12 +529,6 @@
     <t>Sin novedad</t>
   </si>
   <si>
-    <t>5/31/24 12:10:24</t>
-  </si>
-  <si>
-    <t>5/31/24 12:13:14</t>
-  </si>
-  <si>
     <t>nafonsecam@pedagogica.edu.co</t>
   </si>
   <si>
@@ -675,12 +565,6 @@
     <t>Alex</t>
   </si>
   <si>
-    <t>6/14/24 15:19:24</t>
-  </si>
-  <si>
-    <t>6/14/24 15:21:27</t>
-  </si>
-  <si>
     <t>jovenesalau@upn.edu.co</t>
   </si>
   <si>
@@ -696,18 +580,9 @@
     <t xml:space="preserve">Carmen cristina rueda </t>
   </si>
   <si>
-    <t>6/14/2024</t>
-  </si>
-  <si>
     <t>William Hernando Ramírez Contreras</t>
   </si>
   <si>
-    <t>6/14/24 20:33:59</t>
-  </si>
-  <si>
-    <t>6/14/24 20:36:40</t>
-  </si>
-  <si>
     <t>smtorres@pedagogica.edu.co</t>
   </si>
   <si>
@@ -726,21 +601,9 @@
     <t>Gracias por el apoyo</t>
   </si>
   <si>
-    <t>6/21/24 19:47:13</t>
-  </si>
-  <si>
-    <t>6/21/24 19:47:38</t>
-  </si>
-  <si>
     <t>anonymous</t>
   </si>
   <si>
-    <t>6/21/24 19:48:45</t>
-  </si>
-  <si>
-    <t>6/21/24 19:53:43</t>
-  </si>
-  <si>
     <t>Docente Catedrático</t>
   </si>
   <si>
@@ -750,340 +613,56 @@
     <t>Ricardo Torres</t>
   </si>
   <si>
-    <t>6/13/2024</t>
-  </si>
-  <si>
     <t>Sería de suma utilidad para la división de transportes, contar con un furgón para servicios específicos.</t>
   </si>
   <si>
-    <t>6/22/24 19:29:19</t>
-  </si>
-  <si>
-    <t>6/22/24 19:59:56</t>
+    <t>Supernumerario</t>
+  </si>
+  <si>
+    <t>Gladys Cortes</t>
+  </si>
+  <si>
+    <t>Jorge Enrique Mogollón Montañez</t>
+  </si>
+  <si>
+    <t>Huele a gasolina.</t>
+  </si>
+  <si>
+    <t>nGREgiPT_k6Tg1M4a_CM6ISJUD-DI7NBoIgAQxXYz_hUMTdPVkhHNklaVjdQQjcyVFZFS0kwNlFTMSQlQCN0PWcu</t>
+  </si>
+  <si>
+    <t>Form1</t>
+  </si>
+  <si>
+    <t>{e23544ea-7b9b-4957-ba48-7e2c5253e036}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1091,211 +670,114 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1308,8 +790,48 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AE29" totalsRowShown="0">
+  <autoFilter ref="A1:AE29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Hora de la última modificación" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Autoriza el tratamiento de sus datos personales consignados en este formulario de asistencia de la Universidad Pedagógica Nacional, con el objetivo de demostrar su participación en el evento o reu..." dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Tipo de Vinculación:" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="¿En qué instalaciones de la UPN (Universidad Pedagógica Nacional) desarrolla sus actividades y/o labores?" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name=" ¿Cuál es su identidad de género?" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿Cuál es su rango de edad?" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="¿A qué grupo poblacional o sector social perteneces?_x000a_" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="¿A qué grupo de pertenencia étnica pertenece?" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="¿A qué unidad o dependencia de la UPN (Universidad Pedagógica Nacional) perteneces?" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Nombre del funcionario responsable del servicio " dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Fecha en que se efectuó el servicio de transporte:" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Tipo de servicio prestado:" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Nombre del Conductor que prestó el servicio" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Estado mecánico de los vehículo" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Limpieza y presentación general de los vehículos" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Comentarios u observaciones sobre la prestación y estado de los vehículos de la entidad" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Amabilidad y cortesía" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Nivel de atención mientras conduce" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Capacidad de comunicación" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Comentarios u observaciones sobre la atención, actitud y comportamiento del conductor" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="¿Se dio cumplimiento de los itinerarios solicitados?" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="¿Se dio cumplimiento de los horarios solicitados?" dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="¿Durante el recorrido se acataron las normas de tránsito?" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="¿Durante el recorrido se presento algún incidente o accidente?" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="¿Recomendaría los servicios del área de transportes a mas miembros de la comunidad de Universitaria?" dataDxfId="1"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Comentarios u observaciones sobre el cumplimiento de aspectos durante la prestación del servicio :" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1319,44 +841,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1403,12 +925,12 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1514,6 +1036,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1522,13 +1051,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1593,45 +1115,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72CA5D3-4F81-42A4-94DB-302AF7084446}">
-  <dimension ref="A1:AE27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="10" max="31" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1665,7 +1174,7 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
@@ -1726,15 +1235,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31">
       <c r="A2">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>45509.646689814814</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45509.651226851849</v>
+      <c r="B2" s="1">
+        <v>45420.646689814799</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45420.651226851798</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -1742,6 +1251,7 @@
       <c r="E2" t="s">
         <v>32</v>
       </c>
+      <c r="F2" s="1"/>
       <c r="G2" t="s">
         <v>33</v>
       </c>
@@ -1769,8 +1279,8 @@
       <c r="O2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="3">
-        <v>45509</v>
+      <c r="P2" s="2">
+        <v>45420</v>
       </c>
       <c r="Q2" t="s">
         <v>42</v>
@@ -1778,26 +1288,26 @@
       <c r="R2" t="s">
         <v>43</v>
       </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
-      <c r="T2">
-        <v>3</v>
+      <c r="S2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="U2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="V2">
-        <v>3</v>
-      </c>
-      <c r="W2">
-        <v>4</v>
-      </c>
-      <c r="X2">
-        <v>3</v>
+      <c r="W2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="Y2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Z2" t="s">
         <v>33</v>
@@ -1809,21 +1319,21 @@
         <v>33</v>
       </c>
       <c r="AC2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31">
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>45509.651319444441</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45509.653784722221</v>
+      <c r="B3" s="1">
+        <v>45420.651319444398</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45420.653784722199</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -1831,6 +1341,7 @@
       <c r="E3" t="s">
         <v>32</v>
       </c>
+      <c r="F3" s="1"/>
       <c r="G3" t="s">
         <v>33</v>
       </c>
@@ -1858,36 +1369,36 @@
       <c r="O3" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="3">
-        <v>45509</v>
+      <c r="P3" s="2">
+        <v>45420</v>
       </c>
       <c r="Q3" t="s">
         <v>42</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3">
-        <v>3</v>
-      </c>
-      <c r="T3">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>3</v>
-      </c>
-      <c r="W3">
-        <v>4</v>
-      </c>
-      <c r="X3">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z3" t="s">
         <v>48</v>
       </c>
-      <c r="Z3" t="s">
-        <v>46</v>
-      </c>
       <c r="AA3" t="s">
         <v>33</v>
       </c>
@@ -1895,24 +1406,24 @@
         <v>33</v>
       </c>
       <c r="AC3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD3" t="s">
         <v>33</v>
       </c>
       <c r="AE3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31">
       <c r="A4">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
+      <c r="B4" s="1">
+        <v>45429.642071759299</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45429.645891203698</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
@@ -1920,6 +1431,7 @@
       <c r="E4" t="s">
         <v>53</v>
       </c>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>33</v>
       </c>
@@ -1947,32 +1459,32 @@
       <c r="O4" t="s">
         <v>58</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="2">
+        <v>45429</v>
+      </c>
+      <c r="Q4" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>60</v>
       </c>
-      <c r="R4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4">
-        <v>5</v>
-      </c>
-      <c r="T4">
-        <v>5</v>
+      <c r="S4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U4" t="s">
         <v>62</v>
       </c>
-      <c r="V4">
-        <v>5</v>
-      </c>
-      <c r="W4">
-        <v>5</v>
-      </c>
-      <c r="X4">
-        <v>5</v>
+      <c r="V4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y4" t="s">
         <v>63</v>
@@ -1996,22 +1508,23 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31">
       <c r="A5">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1">
+        <v>45429.736203703702</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45429.740104166704</v>
+      </c>
+      <c r="D5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" t="s">
         <v>33</v>
       </c>
@@ -2034,81 +1547,82 @@
         <v>39</v>
       </c>
       <c r="N5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="2">
+        <v>45429</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" t="s">
         <v>69</v>
       </c>
-      <c r="O5" t="s">
+      <c r="S5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" t="s">
         <v>70</v>
       </c>
-      <c r="P5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>60</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="V5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y5" t="s">
         <v>71</v>
       </c>
-      <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="Z5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE5" t="s">
         <v>72</v>
       </c>
-      <c r="V5">
-        <v>5</v>
-      </c>
-      <c r="W5">
-        <v>5</v>
-      </c>
-      <c r="X5">
-        <v>5</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31">
       <c r="A6">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1">
+        <v>45430.640902777799</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45430.643078703702</v>
+      </c>
+      <c r="D6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
         <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>79</v>
       </c>
       <c r="I6" t="s">
         <v>35</v>
@@ -2126,40 +1640,40 @@
         <v>39</v>
       </c>
       <c r="N6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P6" s="3">
-        <v>45631</v>
+        <v>77</v>
+      </c>
+      <c r="P6" s="2">
+        <v>45424</v>
       </c>
       <c r="Q6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R6" t="s">
         <v>43</v>
       </c>
-      <c r="S6">
-        <v>5</v>
-      </c>
-      <c r="T6">
-        <v>5</v>
+      <c r="S6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U6" t="s">
-        <v>82</v>
-      </c>
-      <c r="V6">
-        <v>5</v>
-      </c>
-      <c r="W6">
-        <v>5</v>
-      </c>
-      <c r="X6">
-        <v>5</v>
+        <v>78</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Z6" t="s">
         <v>33</v>
@@ -2171,31 +1685,32 @@
         <v>33</v>
       </c>
       <c r="AC6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD6" t="s">
         <v>33</v>
       </c>
       <c r="AE6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31">
       <c r="A7">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
+      <c r="B7" s="1">
+        <v>45430.711631944403</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45430.713495370401</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F7" s="1"/>
       <c r="G7" t="s">
         <v>33</v>
       </c>
@@ -2218,34 +1733,34 @@
         <v>39</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O7" t="s">
-        <v>90</v>
-      </c>
-      <c r="P7" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="P7" s="2">
+        <v>45430</v>
       </c>
       <c r="Q7" t="s">
         <v>42</v>
       </c>
       <c r="R7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S7">
-        <v>5</v>
-      </c>
-      <c r="T7">
-        <v>5</v>
-      </c>
-      <c r="V7">
-        <v>5</v>
-      </c>
-      <c r="W7">
-        <v>5</v>
-      </c>
-      <c r="X7">
-        <v>5</v>
+        <v>49</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z7" t="s">
         <v>33</v>
@@ -2257,33 +1772,34 @@
         <v>33</v>
       </c>
       <c r="AC7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31">
       <c r="A8">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
+      <c r="B8" s="1">
+        <v>45432.479386574101</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45432.481805555602</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" t="s">
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s">
         <v>35</v>
@@ -2301,34 +1817,34 @@
         <v>39</v>
       </c>
       <c r="N8" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="O8" t="s">
-        <v>98</v>
-      </c>
-      <c r="P8" t="s">
-        <v>99</v>
+        <v>89</v>
+      </c>
+      <c r="P8" s="2">
+        <v>45432</v>
       </c>
       <c r="Q8" t="s">
         <v>42</v>
       </c>
       <c r="R8" t="s">
-        <v>100</v>
-      </c>
-      <c r="S8">
-        <v>5</v>
-      </c>
-      <c r="T8">
-        <v>5</v>
-      </c>
-      <c r="V8">
-        <v>5</v>
-      </c>
-      <c r="W8">
-        <v>5</v>
-      </c>
-      <c r="X8">
-        <v>5</v>
+        <v>90</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z8" t="s">
         <v>33</v>
@@ -2340,33 +1856,34 @@
         <v>33</v>
       </c>
       <c r="AC8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31">
       <c r="A9">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>102</v>
+      <c r="B9" s="1">
+        <v>45433.370590277802</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45433.371770833299</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" t="s">
         <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I9" t="s">
         <v>35</v>
@@ -2375,7 +1892,7 @@
         <v>55</v>
       </c>
       <c r="K9" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="L9" t="s">
         <v>38</v>
@@ -2384,34 +1901,34 @@
         <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="O9" t="s">
-        <v>107</v>
-      </c>
-      <c r="P9" t="s">
-        <v>108</v>
+        <v>95</v>
+      </c>
+      <c r="P9" s="2">
+        <v>45433</v>
       </c>
       <c r="Q9" t="s">
         <v>42</v>
       </c>
       <c r="R9" t="s">
-        <v>109</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-      <c r="V9">
-        <v>5</v>
-      </c>
-      <c r="W9">
-        <v>5</v>
-      </c>
-      <c r="X9">
-        <v>5</v>
+        <v>96</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z9" t="s">
         <v>33</v>
@@ -2423,33 +1940,34 @@
         <v>33</v>
       </c>
       <c r="AC9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31">
       <c r="A10">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
+      <c r="B10" s="1">
+        <v>45433.717199074097</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45433.721793981502</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="F10" s="1"/>
       <c r="G10" t="s">
         <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I10" t="s">
         <v>35</v>
@@ -2470,37 +1988,37 @@
         <v>57</v>
       </c>
       <c r="O10" t="s">
-        <v>114</v>
-      </c>
-      <c r="P10" t="s">
-        <v>115</v>
+        <v>99</v>
+      </c>
+      <c r="P10" s="2">
+        <v>45426</v>
       </c>
       <c r="Q10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R10" t="s">
-        <v>116</v>
-      </c>
-      <c r="S10">
-        <v>4</v>
-      </c>
-      <c r="T10">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U10" t="s">
-        <v>117</v>
-      </c>
-      <c r="V10">
-        <v>5</v>
-      </c>
-      <c r="W10">
-        <v>5</v>
-      </c>
-      <c r="X10">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y10" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="Z10" t="s">
         <v>33</v>
@@ -2512,36 +2030,37 @@
         <v>33</v>
       </c>
       <c r="AC10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD10" t="s">
         <v>33</v>
       </c>
       <c r="AE10" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31">
       <c r="A11">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>121</v>
+      <c r="B11" s="1">
+        <v>45435.403252314798</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45435.406932870399</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" t="s">
         <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="I11" t="s">
         <v>35</v>
@@ -2559,37 +2078,37 @@
         <v>39</v>
       </c>
       <c r="N11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>125</v>
-      </c>
-      <c r="P11" t="s">
-        <v>126</v>
+        <v>107</v>
+      </c>
+      <c r="P11" s="2">
+        <v>45435</v>
       </c>
       <c r="Q11" t="s">
         <v>42</v>
       </c>
       <c r="R11" t="s">
-        <v>109</v>
-      </c>
-      <c r="S11">
-        <v>5</v>
-      </c>
-      <c r="T11">
-        <v>5</v>
+        <v>96</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U11" t="s">
-        <v>127</v>
-      </c>
-      <c r="V11">
-        <v>5</v>
-      </c>
-      <c r="W11">
-        <v>5</v>
-      </c>
-      <c r="X11">
-        <v>5</v>
+        <v>108</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z11" t="s">
         <v>33</v>
@@ -2601,33 +2120,34 @@
         <v>33</v>
       </c>
       <c r="AC11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31">
       <c r="A12">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" t="s">
-        <v>129</v>
+      <c r="B12" s="1">
+        <v>45435.699803240699</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45435.702094907399</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="I12" t="s">
         <v>35</v>
@@ -2636,49 +2156,49 @@
         <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="L12" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="M12" t="s">
         <v>39</v>
       </c>
       <c r="N12" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
-        <v>135</v>
-      </c>
-      <c r="P12" t="s">
-        <v>59</v>
+        <v>114</v>
+      </c>
+      <c r="P12" s="2">
+        <v>45429</v>
       </c>
       <c r="Q12" t="s">
         <v>42</v>
       </c>
       <c r="R12" t="s">
-        <v>47</v>
-      </c>
-      <c r="S12">
-        <v>5</v>
-      </c>
-      <c r="T12">
-        <v>5</v>
+        <v>49</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U12" t="s">
-        <v>136</v>
-      </c>
-      <c r="V12">
-        <v>5</v>
-      </c>
-      <c r="W12">
-        <v>4</v>
-      </c>
-      <c r="X12">
-        <v>5</v>
+        <v>115</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y12" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="Z12" t="s">
         <v>33</v>
@@ -2690,31 +2210,32 @@
         <v>33</v>
       </c>
       <c r="AC12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD12" t="s">
         <v>33</v>
       </c>
       <c r="AE12" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31">
       <c r="A13">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" t="s">
-        <v>139</v>
+      <c r="B13" s="1">
+        <v>45436.507997685199</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45436.509895833296</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>141</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F13" s="1"/>
       <c r="G13" t="s">
         <v>33</v>
       </c>
@@ -2740,37 +2261,37 @@
         <v>57</v>
       </c>
       <c r="O13" t="s">
-        <v>142</v>
-      </c>
-      <c r="P13" t="s">
-        <v>108</v>
+        <v>119</v>
+      </c>
+      <c r="P13" s="2">
+        <v>45433</v>
       </c>
       <c r="Q13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R13" t="s">
-        <v>71</v>
-      </c>
-      <c r="S13">
-        <v>5</v>
-      </c>
-      <c r="T13">
-        <v>5</v>
-      </c>
-      <c r="U13" t="s">
-        <v>143</v>
-      </c>
-      <c r="V13">
-        <v>5</v>
-      </c>
-      <c r="W13">
-        <v>5</v>
-      </c>
-      <c r="X13">
-        <v>5</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>143</v>
+        <v>69</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="Z13" t="s">
         <v>33</v>
@@ -2782,36 +2303,37 @@
         <v>33</v>
       </c>
       <c r="AC13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD13" t="s">
         <v>33</v>
       </c>
-      <c r="AE13" t="s">
-        <v>143</v>
+      <c r="AE13" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31">
       <c r="A14">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C14" t="s">
-        <v>145</v>
+      <c r="B14" s="1">
+        <v>45436.522847222201</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45436.525381944397</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" t="s">
         <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I14" t="s">
         <v>35</v>
@@ -2829,34 +2351,34 @@
         <v>39</v>
       </c>
       <c r="N14" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="O14" t="s">
-        <v>149</v>
-      </c>
-      <c r="P14" t="s">
-        <v>150</v>
+        <v>124</v>
+      </c>
+      <c r="P14" s="2">
+        <v>45436</v>
       </c>
       <c r="Q14" t="s">
         <v>42</v>
       </c>
       <c r="R14" t="s">
-        <v>109</v>
-      </c>
-      <c r="S14">
-        <v>5</v>
-      </c>
-      <c r="T14">
-        <v>5</v>
-      </c>
-      <c r="V14">
-        <v>5</v>
-      </c>
-      <c r="W14">
-        <v>5</v>
-      </c>
-      <c r="X14">
-        <v>5</v>
+        <v>96</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z14" t="s">
         <v>33</v>
@@ -2868,33 +2390,34 @@
         <v>33</v>
       </c>
       <c r="AC14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31">
       <c r="A15">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" t="s">
-        <v>152</v>
+      <c r="B15" s="1">
+        <v>45440.417349536998</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45440.422939814802</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>154</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F15" s="1"/>
       <c r="G15" t="s">
         <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="I15" t="s">
         <v>35</v>
@@ -2912,34 +2435,34 @@
         <v>39</v>
       </c>
       <c r="N15" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="O15" t="s">
-        <v>156</v>
-      </c>
-      <c r="P15" t="s">
-        <v>157</v>
+        <v>128</v>
+      </c>
+      <c r="P15" s="2">
+        <v>45428</v>
       </c>
       <c r="Q15" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="R15" t="s">
-        <v>159</v>
-      </c>
-      <c r="S15">
-        <v>5</v>
-      </c>
-      <c r="T15">
-        <v>5</v>
-      </c>
-      <c r="V15">
-        <v>5</v>
-      </c>
-      <c r="W15">
-        <v>5</v>
-      </c>
-      <c r="X15">
-        <v>5</v>
+        <v>130</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z15" t="s">
         <v>33</v>
@@ -2951,28 +2474,29 @@
         <v>33</v>
       </c>
       <c r="AC15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31">
       <c r="A16">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" t="s">
-        <v>161</v>
+      <c r="B16" s="1">
+        <v>45441.772291666697</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45441.777604166702</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F16" s="1"/>
       <c r="G16" t="s">
         <v>33</v>
       </c>
@@ -2980,7 +2504,7 @@
         <v>54</v>
       </c>
       <c r="I16" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="J16" t="s">
         <v>55</v>
@@ -2995,40 +2519,40 @@
         <v>39</v>
       </c>
       <c r="N16" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="O16" t="s">
-        <v>166</v>
-      </c>
-      <c r="P16" t="s">
-        <v>167</v>
+        <v>135</v>
+      </c>
+      <c r="P16" s="2">
+        <v>45441</v>
       </c>
       <c r="Q16" t="s">
+        <v>59</v>
+      </c>
+      <c r="R16" t="s">
         <v>60</v>
       </c>
-      <c r="R16" t="s">
-        <v>61</v>
-      </c>
-      <c r="S16">
-        <v>4</v>
-      </c>
-      <c r="T16">
-        <v>4</v>
+      <c r="S16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="U16" t="s">
-        <v>168</v>
-      </c>
-      <c r="V16">
-        <v>5</v>
-      </c>
-      <c r="W16">
-        <v>5</v>
-      </c>
-      <c r="X16">
-        <v>5</v>
+        <v>136</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y16" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="Z16" t="s">
         <v>33</v>
@@ -3046,25 +2570,26 @@
         <v>33</v>
       </c>
       <c r="AE16" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31">
       <c r="A17">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" t="s">
-        <v>171</v>
+      <c r="B17" s="1">
+        <v>45442.531759259298</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45442.535706018498</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
-        <v>173</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F17" s="1"/>
       <c r="G17" t="s">
         <v>33</v>
       </c>
@@ -3072,7 +2597,7 @@
         <v>54</v>
       </c>
       <c r="I17" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="J17" t="s">
         <v>36</v>
@@ -3087,40 +2612,40 @@
         <v>39</v>
       </c>
       <c r="N17" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="O17" t="s">
-        <v>176</v>
-      </c>
-      <c r="P17" t="s">
-        <v>177</v>
+        <v>142</v>
+      </c>
+      <c r="P17" s="2">
+        <v>45442</v>
       </c>
       <c r="Q17" t="s">
         <v>42</v>
       </c>
       <c r="R17" t="s">
-        <v>116</v>
-      </c>
-      <c r="S17">
-        <v>5</v>
-      </c>
-      <c r="T17">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U17" t="s">
-        <v>178</v>
-      </c>
-      <c r="V17">
-        <v>5</v>
-      </c>
-      <c r="W17">
-        <v>5</v>
-      </c>
-      <c r="X17">
-        <v>4</v>
+        <v>143</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="Y17" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="Z17" t="s">
         <v>33</v>
@@ -3132,39 +2657,40 @@
         <v>33</v>
       </c>
       <c r="AC17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD17" t="s">
         <v>33</v>
       </c>
       <c r="AE17" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31">
       <c r="A18">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>181</v>
-      </c>
-      <c r="C18" t="s">
-        <v>182</v>
+      <c r="B18" s="1">
+        <v>45442.584305555603</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45442.585972222201</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>146</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="F18" s="1"/>
       <c r="G18" t="s">
         <v>33</v>
       </c>
       <c r="H18" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="J18" t="s">
         <v>55</v>
@@ -3179,37 +2705,37 @@
         <v>39</v>
       </c>
       <c r="N18" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="O18" t="s">
-        <v>186</v>
-      </c>
-      <c r="P18" t="s">
-        <v>177</v>
+        <v>149</v>
+      </c>
+      <c r="P18" s="2">
+        <v>45442</v>
       </c>
       <c r="Q18" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="R18" t="s">
-        <v>159</v>
-      </c>
-      <c r="S18">
-        <v>5</v>
-      </c>
-      <c r="T18">
-        <v>5</v>
+        <v>130</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U18" t="s">
-        <v>187</v>
-      </c>
-      <c r="V18">
-        <v>5</v>
-      </c>
-      <c r="W18">
-        <v>5</v>
-      </c>
-      <c r="X18">
-        <v>5</v>
+        <v>150</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z18" t="s">
         <v>33</v>
@@ -3221,36 +2747,37 @@
         <v>33</v>
       </c>
       <c r="AC18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31">
       <c r="A19">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>188</v>
-      </c>
-      <c r="C19" t="s">
-        <v>189</v>
+      <c r="B19" s="1">
+        <v>45443.458449074104</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45443.459930555597</v>
       </c>
       <c r="D19" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" t="s">
         <v>33</v>
       </c>
       <c r="H19" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I19" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="J19" t="s">
         <v>36</v>
@@ -3265,40 +2792,40 @@
         <v>39</v>
       </c>
       <c r="N19" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="O19" t="s">
-        <v>192</v>
-      </c>
-      <c r="P19" t="s">
-        <v>193</v>
+        <v>153</v>
+      </c>
+      <c r="P19" s="2">
+        <v>45443</v>
       </c>
       <c r="Q19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R19" t="s">
-        <v>116</v>
-      </c>
-      <c r="S19">
-        <v>5</v>
-      </c>
-      <c r="T19">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U19" t="s">
-        <v>168</v>
-      </c>
-      <c r="V19">
-        <v>5</v>
-      </c>
-      <c r="W19">
-        <v>5</v>
-      </c>
-      <c r="X19">
-        <v>5</v>
+        <v>136</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y19" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="Z19" t="s">
         <v>33</v>
@@ -3307,39 +2834,40 @@
         <v>33</v>
       </c>
       <c r="AB19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AC19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD19" t="s">
         <v>33</v>
       </c>
       <c r="AE19" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31">
       <c r="A20">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>195</v>
-      </c>
-      <c r="C20" t="s">
-        <v>196</v>
+      <c r="B20" s="1">
+        <v>45443.496319444399</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45443.5</v>
       </c>
       <c r="D20" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>33</v>
       </c>
       <c r="H20" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I20" t="s">
         <v>35</v>
@@ -3357,40 +2885,40 @@
         <v>39</v>
       </c>
       <c r="N20" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="O20" t="s">
-        <v>199</v>
-      </c>
-      <c r="P20" t="s">
-        <v>193</v>
+        <v>157</v>
+      </c>
+      <c r="P20" s="2">
+        <v>45443</v>
       </c>
       <c r="Q20" t="s">
         <v>42</v>
       </c>
       <c r="R20" t="s">
-        <v>109</v>
-      </c>
-      <c r="S20">
-        <v>5</v>
-      </c>
-      <c r="T20">
-        <v>5</v>
+        <v>96</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U20" t="s">
-        <v>200</v>
-      </c>
-      <c r="V20">
-        <v>5</v>
-      </c>
-      <c r="W20">
-        <v>5</v>
-      </c>
-      <c r="X20">
-        <v>5</v>
+        <v>158</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y20" t="s">
-        <v>201</v>
+        <v>159</v>
       </c>
       <c r="Z20" t="s">
         <v>33</v>
@@ -3408,30 +2936,31 @@
         <v>33</v>
       </c>
       <c r="AE20" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31">
       <c r="A21">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>203</v>
-      </c>
-      <c r="C21" t="s">
-        <v>204</v>
+      <c r="B21" s="1">
+        <v>45443.507222222201</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45443.509189814802</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="E21" t="s">
-        <v>206</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" t="s">
         <v>33</v>
       </c>
       <c r="H21" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="I21" t="s">
         <v>35</v>
@@ -3449,37 +2978,37 @@
         <v>39</v>
       </c>
       <c r="N21" t="s">
-        <v>208</v>
+        <v>164</v>
       </c>
       <c r="O21" t="s">
-        <v>209</v>
-      </c>
-      <c r="P21" t="s">
-        <v>193</v>
+        <v>165</v>
+      </c>
+      <c r="P21" s="2">
+        <v>45443</v>
       </c>
       <c r="Q21" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="R21" t="s">
-        <v>210</v>
-      </c>
-      <c r="S21">
-        <v>5</v>
-      </c>
-      <c r="T21">
-        <v>5</v>
+        <v>166</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U21" t="s">
-        <v>211</v>
-      </c>
-      <c r="V21">
-        <v>5</v>
-      </c>
-      <c r="W21">
-        <v>5</v>
-      </c>
-      <c r="X21">
-        <v>5</v>
+        <v>167</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z21" t="s">
         <v>33</v>
@@ -3497,27 +3026,28 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31">
       <c r="A22">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
-        <v>45297.755497685182</v>
-      </c>
-      <c r="C22" s="2">
-        <v>45297.757094907407</v>
+      <c r="B22" s="1">
+        <v>45444.755497685197</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45444.7570949074</v>
       </c>
       <c r="D22" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="E22" t="s">
-        <v>213</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" t="s">
         <v>33</v>
       </c>
       <c r="H22" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="I22" t="s">
         <v>35</v>
@@ -3526,7 +3056,7 @@
         <v>36</v>
       </c>
       <c r="K22" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="L22" t="s">
         <v>38</v>
@@ -3535,84 +3065,85 @@
         <v>39</v>
       </c>
       <c r="N22" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="O22" t="s">
-        <v>216</v>
-      </c>
-      <c r="P22" s="3">
-        <v>45297</v>
+        <v>172</v>
+      </c>
+      <c r="P22" s="2">
+        <v>45444</v>
       </c>
       <c r="Q22" t="s">
         <v>42</v>
       </c>
       <c r="R22" t="s">
+        <v>100</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U22" t="s">
+        <v>108</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y22" t="s">
         <v>116</v>
       </c>
-      <c r="S22">
-        <v>5</v>
-      </c>
-      <c r="T22">
-        <v>5</v>
-      </c>
-      <c r="U22" t="s">
-        <v>127</v>
-      </c>
-      <c r="V22">
-        <v>5</v>
-      </c>
-      <c r="W22">
-        <v>5</v>
-      </c>
-      <c r="X22">
-        <v>5</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>137</v>
-      </c>
       <c r="Z22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AA22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AB22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AC22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AE22" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31">
       <c r="A23">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>217</v>
-      </c>
-      <c r="C23" t="s">
-        <v>218</v>
+      <c r="B23" s="1">
+        <v>45457.638472222221</v>
+      </c>
+      <c r="C23" s="1">
+        <v>45457.63989583333</v>
       </c>
       <c r="D23" t="s">
-        <v>219</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
-        <v>220</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" t="s">
         <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I23" t="s">
-        <v>221</v>
+        <v>175</v>
       </c>
       <c r="J23" t="s">
         <v>36</v>
@@ -3627,34 +3158,34 @@
         <v>39</v>
       </c>
       <c r="N23" t="s">
-        <v>222</v>
+        <v>176</v>
       </c>
       <c r="O23" t="s">
-        <v>223</v>
-      </c>
-      <c r="P23" t="s">
-        <v>224</v>
+        <v>177</v>
+      </c>
+      <c r="P23" s="2">
+        <v>45457</v>
       </c>
       <c r="Q23" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="R23" t="s">
-        <v>225</v>
-      </c>
-      <c r="S23">
-        <v>5</v>
-      </c>
-      <c r="T23">
-        <v>5</v>
-      </c>
-      <c r="V23">
-        <v>5</v>
-      </c>
-      <c r="W23">
-        <v>5</v>
-      </c>
-      <c r="X23">
-        <v>5</v>
+        <v>178</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X23" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z23" t="s">
         <v>33</v>
@@ -3666,33 +3197,34 @@
         <v>33</v>
       </c>
       <c r="AC23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31">
       <c r="A24">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
-        <v>226</v>
-      </c>
-      <c r="C24" t="s">
-        <v>227</v>
+      <c r="B24" s="1">
+        <v>45457.856932870367</v>
+      </c>
+      <c r="C24" s="1">
+        <v>45457.858796296299</v>
       </c>
       <c r="D24" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>229</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="F24" s="1"/>
       <c r="G24" t="s">
         <v>33</v>
       </c>
       <c r="H24" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="I24" t="s">
         <v>35</v>
@@ -3710,40 +3242,40 @@
         <v>39</v>
       </c>
       <c r="N24" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O24" t="s">
-        <v>231</v>
-      </c>
-      <c r="P24" t="s">
-        <v>224</v>
+        <v>182</v>
+      </c>
+      <c r="P24" s="2">
+        <v>45457</v>
       </c>
       <c r="Q24" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="R24" t="s">
-        <v>116</v>
-      </c>
-      <c r="S24">
-        <v>5</v>
-      </c>
-      <c r="T24">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="U24" t="s">
-        <v>211</v>
-      </c>
-      <c r="V24">
-        <v>5</v>
-      </c>
-      <c r="W24">
-        <v>5</v>
-      </c>
-      <c r="X24">
-        <v>5</v>
+        <v>167</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Y24" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="Z24" t="s">
         <v>33</v>
@@ -3755,50 +3287,58 @@
         <v>33</v>
       </c>
       <c r="AC24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD24" t="s">
         <v>33</v>
       </c>
       <c r="AE24" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31">
       <c r="A25">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
-        <v>234</v>
-      </c>
-      <c r="C25" t="s">
-        <v>235</v>
+      <c r="B25" s="1">
+        <v>45464.824456018519</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45464.824745370373</v>
       </c>
       <c r="D25" t="s">
-        <v>236</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F25" s="1"/>
       <c r="G25" t="s">
-        <v>46</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31">
       <c r="A26">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
-        <v>237</v>
-      </c>
-      <c r="C26" t="s">
-        <v>238</v>
+      <c r="B26" s="1">
+        <v>45464.825520833336</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45464.828969907408</v>
       </c>
       <c r="D26" t="s">
-        <v>236</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F26" s="1"/>
       <c r="G26" t="s">
         <v>33</v>
       </c>
       <c r="H26" t="s">
-        <v>239</v>
+        <v>186</v>
       </c>
       <c r="I26" t="s">
         <v>35</v>
@@ -3816,34 +3356,34 @@
         <v>39</v>
       </c>
       <c r="N26" t="s">
-        <v>240</v>
+        <v>187</v>
       </c>
       <c r="O26" t="s">
-        <v>241</v>
-      </c>
-      <c r="P26" t="s">
-        <v>242</v>
+        <v>188</v>
+      </c>
+      <c r="P26" s="2">
+        <v>45456</v>
       </c>
       <c r="Q26" t="s">
         <v>42</v>
       </c>
       <c r="R26" t="s">
-        <v>61</v>
-      </c>
-      <c r="S26">
-        <v>5</v>
-      </c>
-      <c r="T26">
-        <v>5</v>
-      </c>
-      <c r="V26">
-        <v>5</v>
-      </c>
-      <c r="W26">
-        <v>5</v>
-      </c>
-      <c r="X26">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="Z26" t="s">
         <v>33</v>
@@ -3855,51 +3395,256 @@
         <v>33</v>
       </c>
       <c r="AC26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AD26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AE26" t="s">
-        <v>243</v>
+        <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31">
       <c r="A27">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>244</v>
-      </c>
-      <c r="C27" t="s">
-        <v>245</v>
+      <c r="B27" s="1">
+        <v>45465.812025462961</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45465.833287037036</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+    </row>
+    <row r="28" spans="1:31">
+      <c r="A28">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45470.439201388886</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45470.441643518519</v>
+      </c>
+      <c r="D28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" t="s">
+        <v>190</v>
+      </c>
+      <c r="I28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M28" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" t="s">
+        <v>88</v>
+      </c>
+      <c r="O28" t="s">
+        <v>191</v>
+      </c>
+      <c r="P28" s="2">
+        <v>45470</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>42</v>
+      </c>
+      <c r="R28" t="s">
+        <v>90</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45470.441689814812</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45470.444293981483</v>
+      </c>
+      <c r="D29" t="s">
+        <v>185</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" t="s">
+        <v>190</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" t="s">
+        <v>38</v>
+      </c>
+      <c r="M29" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" t="s">
+        <v>88</v>
+      </c>
+      <c r="O29" t="s">
+        <v>191</v>
+      </c>
+      <c r="P29" s="2">
+        <v>45470</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>42</v>
+      </c>
+      <c r="R29" t="s">
+        <v>192</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U29" t="s">
+        <v>193</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042DEF5FC94E91D4EB00C55EFAF062246" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aae3622a3a9c19db123ec536fce947b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a10e06ba-394c-4d9b-8c5d-aa5df1cb575e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d2b6021f0e0080b66ae9e08b66535c9" ns3:_="">
-    <xsd:import namespace="a10e06ba-394c-4d9b-8c5d-aa5df1cb575e"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D45681223310045808A22EA47D7845F" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="9b9450793f3d36e97df90e069ade6c5b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0c2a4331-f396-4bb5-9ba8-7f95892487d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d9c68a369494e1f3cefcf3e5a9d305c" ns2:_="">
+    <xsd:import namespace="0c2a4331-f396-4bb5-9ba8-7f95892487d8"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3907,7 +3652,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a10e06ba-394c-4d9b-8c5d-aa5df1cb575e" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0c2a4331-f396-4bb5-9ba8-7f95892487d8" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -3940,8 +3685,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -4031,6 +3776,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4039,50 +3790,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE38AED-7BD5-41C2-90FC-B98B21F947D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a10e06ba-394c-4d9b-8c5d-aa5df1cb575e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9B834CB-30B8-47F7-828A-C420AC525921}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B73261C2-8B76-48B6-8514-B1CD46BED53B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F94192-ACE3-4F6C-BC44-CE65402515D2}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFEBAC79-D124-4D7B-8738-B95A45E9A5D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a10e06ba-394c-4d9b-8c5d-aa5df1cb575e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3319C442-CA14-4432-988E-65269E15CEAF}"/>
 </file>
</xml_diff>